<commit_message>
Assault weapons and such
</commit_message>
<xml_diff>
--- a/data/aid.xlsx
+++ b/data/aid.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Repos/savagewasteland/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1D0F32-2051-BF42-815C-5A03E603EEDF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7BE44B-051E-1849-9527-3767723DC3B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29820" windowHeight="17140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Qty</t>
   </si>
@@ -84,9 +90,6 @@
     <t>Hydra</t>
   </si>
   <si>
-    <t>Inject as an action.  If applied to wound or perminant injury, subject makes vigor roll.  Success causes injury to heal over 1d6 hours.</t>
-  </si>
-  <si>
     <t>⅒</t>
   </si>
   <si>
@@ -102,20 +105,104 @@
     <t>Rad Away</t>
   </si>
   <si>
-    <t>Inject via IV (1 minute).   For four hours, subject experiences -1 vigor rolls and requires additional day's water.  After four hours, one level of radiation exposure is removed.</t>
-  </si>
-  <si>
     <t>Drink as an action. | Effects: +1 Spirit, -1 Agility, -1 Smarts for 1 hour. | Alcohol stacks up to x2, then adds +1 hour per additional dose. | Hangover: -1 Spirit, -1 Smarts for (2x dose - vigor roll) hours. | Addictive.</t>
   </si>
   <si>
     <t>Inject as an action. | Healing or Common Knowledge check at +2. | Failure removes shaken, success removes shaken and one wound, each raise removes 1 wound per turn.</t>
+  </si>
+  <si>
+    <t>Rad-X</t>
+  </si>
+  <si>
+    <t>Inject via IV (1 minute).  For four hours, subject experiences -1 vigor rolls and requires additional day's water.  After four hours, one level of radiation exposure is removed.</t>
+  </si>
+  <si>
+    <t>Inject via IV (1 minute).  If applied to wound or perminant injury, subject makes vigor roll, which can be assisted by healing roll.  Success causes injury to heal over 1d6 hours.</t>
+  </si>
+  <si>
+    <t>Bloatfly Meat</t>
+  </si>
+  <si>
+    <t>Buffout</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Cram</t>
+  </si>
+  <si>
+    <t>Dandy Boy Apples</t>
+  </si>
+  <si>
+    <t>Fancy Lad Snack Cakes</t>
+  </si>
+  <si>
+    <t>Mentats</t>
+  </si>
+  <si>
+    <t>Molerat Meat</t>
+  </si>
+  <si>
+    <t>Mutfruit</t>
+  </si>
+  <si>
+    <t>Radroach Meat</t>
+  </si>
+  <si>
+    <t>Radscorpion Steak</t>
+  </si>
+  <si>
+    <t>Sugar Bombs</t>
+  </si>
+  <si>
+    <t>Vodka</t>
+  </si>
+  <si>
+    <t>Whiskey</t>
+  </si>
+  <si>
+    <t>Ingest pill as an action.  For 4 hours, gain +1 to Strength and Vigor and all Strength related skills.  After 4 hours, withdrawl causes -1 to Strength and Vigor and all Strength related skills. | Addictive</t>
+  </si>
+  <si>
+    <t>Ingest pill as an action.  For 24 hours, gain +1 to Smarts and all Smarts related skills. | Addictive.</t>
+  </si>
+  <si>
+    <t>Ingest pill as an action.  For four hours, time required to absorb one radiation level is increased one step. [1 Turn / 5 Min / 4 Hour / 1 Week / 1 Year]</t>
+  </si>
+  <si>
+    <t>Nomnom</t>
+  </si>
+  <si>
+    <t>Counts as 1/4 day's food.  Useful cooking ingredient</t>
+  </si>
+  <si>
+    <t>Counts as 1/4's day's food.  Mutated carrots grow large in the south.  Useful cooking ingredient.</t>
+  </si>
+  <si>
+    <t>Salty and bland, but packed with protein.  Counts as one day's food.  Can be eaten raw or further cooked</t>
+  </si>
+  <si>
+    <t>½</t>
+  </si>
+  <si>
+    <t>Requires cooking.  Counts as 1/2 day's food.  Somehow both mushy and stringy.</t>
+  </si>
+  <si>
+    <t>Sticky sugary apples.  Counts as 1/2 day's food.  Not very nutitious but very tasty.</t>
+  </si>
+  <si>
+    <t>Lots of little sugary cakes.  Each dose counts as 1/2 day's food.  Not very nutritious but very tasty.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +240,14 @@
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -196,7 +291,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -214,6 +309,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -575,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,10 +710,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
         <v>25</v>
@@ -627,24 +725,24 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5">
         <v>20</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -652,7 +750,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
         <v>20</v>
@@ -669,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5">
         <v>20</v>
@@ -683,158 +781,423 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="5">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="D6" s="5">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="D7" s="5">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>80</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
-        <v>250</v>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>400</v>
       </c>
       <c r="D9" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="5">
-        <v>55</v>
-      </c>
-      <c r="D10" s="5">
-        <v>3</v>
+        <v>1500</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E10" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5">
+        <v>10</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>80</v>
-      </c>
-      <c r="D11" s="5" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>20</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5">
+        <v>10</v>
+      </c>
+      <c r="F16" s="7" t="str">
+        <f>F15</f>
+        <v>Drink as an action. | Effects: +1 Spirit, -1 Agility, -1 Smarts for 1 hour. | Alcohol stacks up to x2, then adds +1 hour per additional dose. | Hangover: -1 Spirit, -1 Smarts for (2x dose - vigor roll) hours. | Addictive.</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>15</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>10</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f>F15</f>
+        <v>Drink as an action. | Effects: +1 Spirit, -1 Agility, -1 Smarts for 1 hour. | Alcohol stacks up to x2, then adds +1 hour per additional dose. | Hangover: -1 Spirit, -1 Smarts for (2x dose - vigor roll) hours. | Addictive.</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28"/>
-      <c r="D28" s="6"/>
+      <c r="D22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <v>14</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3">
+        <v>36</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3">
+        <v>5</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>8</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29"/>
-      <c r="D29" s="6"/>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>65</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
       <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30"/>
-      <c r="D30" s="6"/>
+      <c r="F29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3">
+        <v>11</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31"/>
-      <c r="D31" s="6"/>
+      <c r="F30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32"/>
-      <c r="D32" s="6"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33"/>
-      <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
@@ -871,6 +1234,21 @@
       <c r="B40"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -880,4 +1258,137 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C14454-01EC-294A-9DCD-054D0EFCF64E}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="3"/>
+      <c r="D13" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>